<commit_message>
Added combined dataset so dates match
</commit_message>
<xml_diff>
--- a/EUROSTOXX600.xlsx
+++ b/EUROSTOXX600.xlsx
@@ -8,16 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\morit\Documents\School\MSc - Risk Management (Semester 3)\Market-Risk-Covid-Crisis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0C3A031-E227-47B5-B8C1-DEFA0F860A17}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B44E8754-EE29-4F4F-BE21-359AD35E5387}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{09EDC8F4-6006-447F-AD23-4BAB6E3AB820}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{09EDC8F4-6006-447F-AD23-4BAB6E3AB820}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="ExternalData_1" localSheetId="1" hidden="1">Sheet2!$A$1:$B$556</definedName>
+    <definedName name="ExternalData_1" localSheetId="0" hidden="1">Sheet1!$A$1:$B$556</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -1619,7 +1618,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="[$]d\ mmm\ yyyy;@" x16r2:formatCode16="[$-en-DE,1]d\ mmm\ yyyy;@"/>
+    <numFmt numFmtId="164" formatCode="[$]d\ mmm\ yyyy;@" x16r2:formatCode16="[$-en-DE,1]d\ mmm\ yyyy;@"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -1659,17 +1658,17 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
-      <numFmt numFmtId="165" formatCode="[$]d\ mmm\ yyyy;@" x16r2:formatCode16="[$-en-DE,1]d\ mmm\ yyyy;@"/>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt numFmtId="164" formatCode="[$]d\ mmm\ yyyy;@" x16r2:formatCode16="[$-en-DE,1]d\ mmm\ yyyy;@"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1706,8 +1705,8 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{969ADF55-A746-45ED-B37D-F44469A2C3F2}" name="STOXX_600_Historical_Data" displayName="STOXX_600_Historical_Data" ref="A1:B556" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:B556" xr:uid="{85A16B13-C92C-47E0-BEBD-31360AA39BA7}"/>
   <tableColumns count="2">
-    <tableColumn id="8" xr3:uid="{446134CC-4016-425D-93E3-6307E09F824C}" uniqueName="8" name="Date" queryTableFieldId="1" dataDxfId="0"/>
-    <tableColumn id="2" xr3:uid="{31FD3A4C-67BD-4BC8-92C9-97417DABEBA7}" uniqueName="2" name="Price" queryTableFieldId="2" dataDxfId="1"/>
+    <tableColumn id="8" xr3:uid="{446134CC-4016-425D-93E3-6307E09F824C}" uniqueName="8" name="Date" queryTableFieldId="1" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{31FD3A4C-67BD-4BC8-92C9-97417DABEBA7}" uniqueName="2" name="Price" queryTableFieldId="2" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2009,18 +2008,6 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48EDC6FA-CB10-4153-B470-807F51C3DF9F}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F750DB7-6EB2-4DA7-A270-38EF0870F63D}">
   <dimension ref="A1:B556"/>
   <sheetViews>

</xml_diff>